<commit_message>
updates while debugging debugger on vscode
</commit_message>
<xml_diff>
--- a/docs/stmts.xlsx
+++ b/docs/stmts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cygwin64\home\bwg\mtbprojects\basoc-6\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\butch\mtbprojects\basoc-6\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67442A7-3607-4FC7-820B-D1B514FF9BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AAA38F-671C-4745-A2E8-22972CBE108F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="-80" windowWidth="34930" windowHeight="20960" xr2:uid="{0188AC2A-6BD5-439D-B758-B55265231E55}"/>
+    <workbookView xWindow="-31960" yWindow="1560" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{0188AC2A-6BD5-439D-B758-B55265231E55}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
   <si>
     <t>Statement</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>FUNCTION SQRT</t>
+  </si>
+  <si>
+    <t>FNINDEX</t>
   </si>
 </sst>
 </file>
@@ -299,11 +302,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -621,7 +624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C1BC22-8CFC-45E5-BE7B-C08D81F739F5}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -784,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93AF4A0-F72A-4B99-9A91-188FE8B01470}">
   <dimension ref="B1:AA30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -803,29 +806,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
     </row>
     <row r="2" spans="2:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
@@ -1107,21 +1110,21 @@
       <c r="G8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
       <c r="L8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="M8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
       <c r="Q8" s="6" t="s">
         <v>20</v>
       </c>
@@ -1232,9 +1235,18 @@
       <c r="G13" t="s">
         <v>39</v>
       </c>
-      <c r="I13" t="s">
+      <c r="H13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
     </row>
     <row r="17" spans="7:23" x14ac:dyDescent="0.35">
       <c r="K17" s="3"/>
@@ -1260,7 +1272,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="20">
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="T7:W7"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="H13:K13"/>
     <mergeCell ref="H9:K9"/>
     <mergeCell ref="L9:O9"/>
     <mergeCell ref="H4:K4"/>
@@ -1277,8 +1293,6 @@
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H7:K7"/>
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="T7:W7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more work on debugger issues
</commit_message>
<xml_diff>
--- a/docs/stmts.xlsx
+++ b/docs/stmts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\butch\mtbprojects\basoc-6\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AAA38F-671C-4745-A2E8-22972CBE108F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22AD65F-1FFF-48F0-8F85-FB7E24304A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31960" yWindow="1560" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{0188AC2A-6BD5-439D-B758-B55265231E55}"/>
+    <workbookView xWindow="-34450" yWindow="4410" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{0188AC2A-6BD5-439D-B758-B55265231E55}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="69">
   <si>
     <t>Statement</t>
   </si>
@@ -145,9 +145,6 @@
     <t>END LINE: INT</t>
   </si>
   <si>
-    <t>ssssssssssssssssssssssssssssss</t>
-  </si>
-  <si>
     <t>CLEAR</t>
   </si>
   <si>
@@ -224,13 +221,37 @@
   </si>
   <si>
     <t>FNINDEX</t>
+  </si>
+  <si>
+    <t>Statis</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>FOR</t>
+  </si>
+  <si>
+    <t>BTOKEN_FOR</t>
+  </si>
+  <si>
+    <t>START: EXPRINDEX</t>
+  </si>
+  <si>
+    <t>END:EXPRINDEX</t>
+  </si>
+  <si>
+    <t>STEP:EXPRINDEX</t>
+  </si>
+  <si>
+    <t>NEXT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +283,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -283,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -299,6 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -622,152 +652,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C1BC22-8CFC-45E5-BE7B-C08D81F739F5}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
         <v>47</v>
       </c>
-      <c r="C7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -775,7 +812,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -785,10 +822,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93AF4A0-F72A-4B99-9A91-188FE8B01470}">
-  <dimension ref="B1:AA30"/>
+  <dimension ref="B1:AA23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13:K13"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -806,29 +843,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
     </row>
     <row r="2" spans="2:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
@@ -929,30 +966,30 @@
       <c r="G3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7" t="s">
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7" t="s">
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7" t="s">
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
       <c r="X3" t="s">
         <v>27</v>
       </c>
@@ -976,12 +1013,12 @@
       <c r="G4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
@@ -1002,12 +1039,12 @@
       <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
@@ -1028,18 +1065,18 @@
       <c r="G6" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7" t="s">
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
@@ -1060,36 +1097,36 @@
       <c r="G7" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7" t="s">
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7" t="s">
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7" t="s">
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7" t="s">
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
-      <c r="AA7" s="7"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
     </row>
     <row r="8" spans="2:27" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
@@ -1110,21 +1147,21 @@
       <c r="G8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
       <c r="L8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="M8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
       <c r="Q8" s="6" t="s">
         <v>20</v>
       </c>
@@ -1158,18 +1195,18 @@
       <c r="G9" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7" t="s">
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
@@ -1210,52 +1247,113 @@
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
         <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
         <v>38</v>
       </c>
-      <c r="G13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7" t="s">
+      <c r="H13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-    </row>
-    <row r="17" spans="7:23" x14ac:dyDescent="0.35">
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="9:23" x14ac:dyDescent="0.35">
       <c r="K17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="22" spans="7:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="9:23" x14ac:dyDescent="0.35">
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="7:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="9:23" x14ac:dyDescent="0.35">
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
@@ -1266,19 +1364,8 @@
       <c r="V23" s="4"/>
       <c r="W23" s="4"/>
     </row>
-    <row r="30" spans="7:23" x14ac:dyDescent="0.35">
-      <c r="G30" t="s">
-        <v>35</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="T7:W7"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="L9:O9"/>
+  <mergeCells count="24">
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="G1:AA1"/>
@@ -1293,6 +1380,16 @@
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H7:K7"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="T7:W7"/>
+    <mergeCell ref="P14:S14"/>
+    <mergeCell ref="T14:W14"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:O14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated with work from last night and this morning
</commit_message>
<xml_diff>
--- a/docs/stmts.xlsx
+++ b/docs/stmts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\butch\mtbprojects\basoc-6\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cygwin64\home\bwg\mtbprojects\basoc-6\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22AD65F-1FFF-48F0-8F85-FB7E24304A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76E5263-40DC-4B76-B9F0-CAB801CBE2C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34450" yWindow="4410" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{0188AC2A-6BD5-439D-B758-B55265231E55}"/>
+    <workbookView xWindow="2240" yWindow="-80" windowWidth="34930" windowHeight="20960" xr2:uid="{0188AC2A-6BD5-439D-B758-B55265231E55}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
   <si>
     <t>Statement</t>
   </si>
@@ -181,15 +181,6 @@
     <t>IF/THEN</t>
   </si>
   <si>
-    <t>IF RND(1) &gt; 0.96 THEN B3 = 1</t>
-  </si>
-  <si>
-    <t>Example</t>
-  </si>
-  <si>
-    <t>DEF FNA(B)=2*B</t>
-  </si>
-  <si>
     <t>OPERATOR ^</t>
   </si>
   <si>
@@ -223,9 +214,6 @@
     <t>FNINDEX</t>
   </si>
   <si>
-    <t>Statis</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
@@ -245,6 +233,12 @@
   </si>
   <si>
     <t>NEXT</t>
+  </si>
+  <si>
+    <t>BTOKEN_NEXT</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -654,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C1BC22-8CFC-45E5-BE7B-C08D81F739F5}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,11 +666,9 @@
         <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>48</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
@@ -686,10 +678,7 @@
         <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -699,6 +688,9 @@
       <c r="B3" t="s">
         <v>42</v>
       </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -731,16 +723,13 @@
       <c r="B7" t="s">
         <v>46</v>
       </c>
-      <c r="D7" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -748,7 +737,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -756,7 +745,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -764,7 +753,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -772,7 +761,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -780,7 +769,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -788,7 +777,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -796,7 +785,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -804,7 +793,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -812,7 +801,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -824,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93AF4A0-F72A-4B99-9A91-188FE8B01470}">
   <dimension ref="B1:AA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1285,7 +1274,7 @@
         <v>38</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -1299,7 +1288,7 @@
     </row>
     <row r="14" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
@@ -1314,7 +1303,7 @@
         <v>21</v>
       </c>
       <c r="G14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>12</v>
@@ -1323,19 +1312,19 @@
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
       <c r="T14" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
@@ -1343,7 +1332,22 @@
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>68</v>
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="9:23" x14ac:dyDescent="0.35">
@@ -1366,6 +1370,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="P14:S14"/>
+    <mergeCell ref="T14:W14"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:O14"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="G1:AA1"/>
@@ -1382,14 +1394,6 @@
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="P7:S7"/>
     <mergeCell ref="T7:W7"/>
-    <mergeCell ref="P14:S14"/>
-    <mergeCell ref="T14:W14"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="L9:O9"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="L14:O14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more work on operators
</commit_message>
<xml_diff>
--- a/docs/stmts.xlsx
+++ b/docs/stmts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cygwin64\home\bwg\mtbprojects\basoc-6\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76E5263-40DC-4B76-B9F0-CAB801CBE2C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4742E30E-3CB5-4E0D-9200-3F5B29FB9112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="-80" windowWidth="34930" windowHeight="20960" xr2:uid="{0188AC2A-6BD5-439D-B758-B55265231E55}"/>
+    <workbookView xWindow="-38510" yWindow="-190" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{0188AC2A-6BD5-439D-B758-B55265231E55}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="94">
   <si>
     <t>Statement</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>EXPRINDEX</t>
-  </si>
-  <si>
-    <t>VARINDEX</t>
   </si>
   <si>
     <t>Parse</t>
@@ -106,12 +103,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>DIM1 (INT)</t>
-  </si>
-  <si>
-    <t>DIM2 (INT)</t>
-  </si>
-  <si>
     <t>DIM1:EXPRINDEX</t>
   </si>
   <si>
@@ -169,9 +160,6 @@
     <t>For loops</t>
   </si>
   <si>
-    <t>RND (args?)</t>
-  </si>
-  <si>
     <t>GOTO</t>
   </si>
   <si>
@@ -239,6 +227,99 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>VARNAME: STRIDX</t>
+  </si>
+  <si>
+    <t>DIMCNT: UINT32</t>
+  </si>
+  <si>
+    <t>DIM1: UINT32</t>
+  </si>
+  <si>
+    <t>DIM2: UINT32</t>
+  </si>
+  <si>
+    <t>Better error reporting</t>
+  </si>
+  <si>
+    <t>Parenthesis in basic_operand_to_string</t>
+  </si>
+  <si>
+    <t>BTOKEN_GOTO</t>
+  </si>
+  <si>
+    <t>BTOKEN_GOSUB</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>BTOKEN_RETURN</t>
+  </si>
+  <si>
+    <t>LINENO: INT</t>
+  </si>
+  <si>
+    <t>READ/DATA</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>INPUT</t>
+  </si>
+  <si>
+    <t>FUNCTIONS</t>
+  </si>
+  <si>
+    <t>STATEMENTS</t>
+  </si>
+  <si>
+    <t>TRON</t>
+  </si>
+  <si>
+    <t>TROFF</t>
+  </si>
+  <si>
+    <t>RENAME</t>
+  </si>
+  <si>
+    <t>SQRT(n)</t>
+  </si>
+  <si>
+    <t>ABS(n)</t>
+  </si>
+  <si>
+    <t>ATN(n)</t>
+  </si>
+  <si>
+    <t>COS(n)</t>
+  </si>
+  <si>
+    <t>EXP(n)</t>
+  </si>
+  <si>
+    <t>LOG(n)</t>
+  </si>
+  <si>
+    <t>SIN(n)</t>
+  </si>
+  <si>
+    <t>TAN(n)</t>
+  </si>
+  <si>
+    <t>MID$(s,n,n)</t>
+  </si>
+  <si>
+    <t>RENUMBER</t>
+  </si>
+  <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>BTOKEN_IF</t>
   </si>
 </sst>
 </file>
@@ -286,12 +367,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -306,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -323,6 +410,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -646,166 +734,254 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C1BC22-8CFC-45E5-BE7B-C08D81F739F5}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.81640625" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D1" s="7"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="I1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="I2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" t="s">
+        <v>91</v>
+      </c>
+      <c r="M5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>42</v>
       </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="M6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="M8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="M9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="M11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>56</v>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -813,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93AF4A0-F72A-4B99-9A91-188FE8B01470}">
   <dimension ref="B1:AA23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -832,45 +1008,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
     </row>
     <row r="2" spans="2:27" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
@@ -941,46 +1117,46 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
+      <c r="H3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
       <c r="X3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:27" x14ac:dyDescent="0.35">
@@ -988,171 +1164,171 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
     </row>
     <row r="5" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="8"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
     </row>
     <row r="8" spans="2:27" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
       <c r="L8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
       <c r="Q8" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
@@ -1167,197 +1343,286 @@
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" t="s">
-        <v>32</v>
-      </c>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
     </row>
     <row r="14" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="9:23" x14ac:dyDescent="0.35">
-      <c r="K17" s="3"/>
+        <v>61</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
+        <v>70</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="22" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.35">
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="9:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:23" x14ac:dyDescent="0.35">
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
@@ -1369,15 +1634,11 @@
       <c r="W23" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="P14:S14"/>
-    <mergeCell ref="T14:W14"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="L9:O9"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="L14:O14"/>
+  <mergeCells count="28">
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H17:K17"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="G1:AA1"/>
@@ -1394,6 +1655,14 @@
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="P7:S7"/>
     <mergeCell ref="T7:W7"/>
+    <mergeCell ref="P14:S14"/>
+    <mergeCell ref="T14:W14"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:O14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
bug fixes, added del and rename
</commit_message>
<xml_diff>
--- a/docs/stmts.xlsx
+++ b/docs/stmts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cygwin64\home\bwg\mtbprojects\basoc-6\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4742E30E-3CB5-4E0D-9200-3F5B29FB9112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B3406B-78D7-4327-8254-2AC320AE1775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-190" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{0188AC2A-6BD5-439D-B758-B55265231E55}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="97">
   <si>
     <t>Statement</t>
   </si>
@@ -320,6 +320,15 @@
   </si>
   <si>
     <t>BTOKEN_IF</t>
+  </si>
+  <si>
+    <t>DEL</t>
+  </si>
+  <si>
+    <t>BTOKEN_DEL</t>
+  </si>
+  <si>
+    <t>BTOKEN_RENAME</t>
   </si>
 </sst>
 </file>
@@ -990,7 +999,7 @@
   <dimension ref="B1:AA23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19:K19"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1609,6 +1618,18 @@
       <c r="B19" t="s">
         <v>92</v>
       </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
       <c r="G19" t="s">
         <v>93</v>
       </c>
@@ -1618,6 +1639,64 @@
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" t="s">
+        <v>96</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.35">
       <c r="I22" s="4"/>
@@ -1634,13 +1713,18 @@
       <c r="W23" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="H5:K5"/>
+  <mergeCells count="31">
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="L21:O21"/>
+    <mergeCell ref="P14:S14"/>
+    <mergeCell ref="T14:W14"/>
+    <mergeCell ref="L13:O13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:O10"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:O14"/>
     <mergeCell ref="G1:AA1"/>
     <mergeCell ref="X7:AA7"/>
     <mergeCell ref="H8:K8"/>
@@ -1655,14 +1739,12 @@
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="P7:S7"/>
     <mergeCell ref="T7:W7"/>
-    <mergeCell ref="P14:S14"/>
-    <mergeCell ref="T14:W14"/>
-    <mergeCell ref="L13:O13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:O10"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="H5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more work on bug fixes
</commit_message>
<xml_diff>
--- a/docs/stmts.xlsx
+++ b/docs/stmts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cygwin64\home\bwg\mtbprojects\basoc-6\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B3406B-78D7-4327-8254-2AC320AE1775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCE2764-547B-491D-9355-5E23783B5A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-190" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{0188AC2A-6BD5-439D-B758-B55265231E55}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{0188AC2A-6BD5-439D-B758-B55265231E55}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="107">
   <si>
     <t>Statement</t>
   </si>
@@ -329,6 +329,36 @@
   </si>
   <si>
     <t>BTOKEN_RENAME</t>
+  </si>
+  <si>
+    <t>BTOKEN_INPUT</t>
+  </si>
+  <si>
+    <t>ON/GOTO</t>
+  </si>
+  <si>
+    <t>BTOKEN_ON</t>
+  </si>
+  <si>
+    <t>LINENO:INT</t>
+  </si>
+  <si>
+    <t>etc</t>
+  </si>
+  <si>
+    <t>ON/GOSUB</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>BTOKEN_END</t>
+  </si>
+  <si>
+    <t>STOP</t>
+  </si>
+  <si>
+    <t>BTOKEN_PROMPT/BTOKEN_NO_PROMPT</t>
   </si>
 </sst>
 </file>
@@ -996,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93AF4A0-F72A-4B99-9A91-188FE8B01470}">
-  <dimension ref="B1:AA23"/>
+  <dimension ref="B1:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="H22" sqref="H22:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1007,7 +1037,7 @@
     <col min="2" max="2" width="14.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="12.1796875" customWidth="1"/>
     <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7265625" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.453125" customWidth="1"/>
     <col min="11" max="11" width="6.7265625" customWidth="1"/>
     <col min="12" max="12" width="23.08984375" customWidth="1"/>
@@ -1699,10 +1729,58 @@
       <c r="O21" s="9"/>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="I22" s="4"/>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="O23" s="4"/>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>97</v>
+      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
@@ -1712,19 +1790,161 @@
       <c r="V23" s="4"/>
       <c r="W23" s="4"/>
     </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" t="s">
+        <v>99</v>
+      </c>
+      <c r="H24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>99</v>
+      </c>
+      <c r="H25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="40">
+    <mergeCell ref="I25:L25"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="Q25:T25"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="I24:L24"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="Q24:T24"/>
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="H21:K21"/>
     <mergeCell ref="L21:O21"/>
     <mergeCell ref="P14:S14"/>
     <mergeCell ref="T14:W14"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="T7:W7"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="H5:K5"/>
     <mergeCell ref="L13:O13"/>
     <mergeCell ref="H13:K13"/>
     <mergeCell ref="H10:K10"/>
     <mergeCell ref="L10:O10"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="H23:K23"/>
     <mergeCell ref="G1:AA1"/>
     <mergeCell ref="X7:AA7"/>
     <mergeCell ref="H8:K8"/>
@@ -1737,14 +1957,6 @@
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="L6:O6"/>
     <mergeCell ref="H7:K7"/>
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="T7:W7"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="H5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>